<commit_message>
Finished Q Measurement Fix!
</commit_message>
<xml_diff>
--- a/Files to Fix/D9K262.00Z.04_RIG_M2aC6_vctrl_sweep.xlsx
+++ b/Files to Fix/D9K262.00Z.04_RIG_M2aC6_vctrl_sweep.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Engineering\Projects\Rigel\Engineering Test\Phase4_Rigel2C_CSP\D9K262.00Z w.04_Rigel2C_CSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler.walker\Documents\Workspace\Python\Wafter4_x-y_Fix\Wafter4_x-y_Fix\Files to Fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1AB833D1-D93F-4F4B-912B-660B67B69559}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F56180-DDB2-4DB1-B90F-C5C97F03F04B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D9K262.00Z.04_RIG_M2aC6_vctrl_s" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'D9K262.00Z.04_RIG_M2aC6_vctrl_s'!$A$1:$T$217</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -97,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -931,11 +934,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+      <selection activeCell="G222" sqref="G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1044258330</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>5.5180583680000002</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1044258330</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>5.5062196080000003</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1044258330</v>
       </c>
@@ -1191,7 +1195,7 @@
         <v>5.5373575009999998</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1044258587</v>
       </c>
@@ -1253,7 +1257,7 @@
         <v>7.1555810319999997</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1044258587</v>
       </c>
@@ -1315,7 +1319,7 @@
         <v>7.1793726510000004</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1044258587</v>
       </c>
@@ -1377,7 +1381,7 @@
         <v>7.2006097860000002</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1439,7 +1443,7 @@
         <v>5.2891458780000002</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1501,7 +1505,7 @@
         <v>5.2027268070000003</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1563,7 +1567,7 @@
         <v>5.3503994429999997</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1044260643</v>
       </c>
@@ -1625,7 +1629,7 @@
         <v>5.2091394150000001</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1044260643</v>
       </c>
@@ -1687,7 +1691,7 @@
         <v>5.0590706719999998</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1044260643</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>5.0696760420000002</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1061035794</v>
       </c>
@@ -1811,7 +1815,7 @@
         <v>4.9111251319999996</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1061035794</v>
       </c>
@@ -1873,7 +1877,7 @@
         <v>4.8461105140000003</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1061035794</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>5.7005592749999998</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1061035802</v>
       </c>
@@ -2183,7 +2187,7 @@
         <v>5.3862320529999996</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1061035802</v>
       </c>
@@ -2245,7 +2249,7 @@
         <v>5.4379812310000002</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1061035802</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>5.263460534</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1061035803</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>6.1457174160000001</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1061035803</v>
       </c>
@@ -2431,7 +2435,7 @@
         <v>6.0889210020000002</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1061035803</v>
       </c>
@@ -2493,7 +2497,7 @@
         <v>5.9766049900000002</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1061039906</v>
       </c>
@@ -2555,7 +2559,7 @@
         <v>5.474817753</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1061039906</v>
       </c>
@@ -2617,7 +2621,7 @@
         <v>5.4383950570000001</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1061039906</v>
       </c>
@@ -2679,7 +2683,7 @@
         <v>5.4016815759999997</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1061039907</v>
       </c>
@@ -2741,7 +2745,7 @@
         <v>4.9597650770000001</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1061039907</v>
       </c>
@@ -2803,7 +2807,7 @@
         <v>4.8934996130000004</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1061039907</v>
       </c>
@@ -2865,7 +2869,7 @@
         <v>4.8526989560000002</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1061039914</v>
       </c>
@@ -2927,7 +2931,7 @@
         <v>5.524576562</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1061039914</v>
       </c>
@@ -2989,7 +2993,7 @@
         <v>5.5255366219999997</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1061039914</v>
       </c>
@@ -3051,7 +3055,7 @@
         <v>5.5460866009999998</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1061039915</v>
       </c>
@@ -3113,7 +3117,7 @@
         <v>5.4711622850000001</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1061039915</v>
       </c>
@@ -3175,7 +3179,7 @@
         <v>5.4079358070000003</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1061039915</v>
       </c>
@@ -3237,7 +3241,7 @@
         <v>5.5027667969999996</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1044258314</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>5.3993914810000003</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1044258314</v>
       </c>
@@ -3361,7 +3365,7 @@
         <v>5.5786511729999999</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1044258314</v>
       </c>
@@ -3423,7 +3427,7 @@
         <v>5.5375776119999998</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1044258571</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>4.7238060409999996</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1044258571</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>4.6385407450000002</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1044258571</v>
       </c>
@@ -3609,7 +3613,7 @@
         <v>4.6527223930000003</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1044256274</v>
       </c>
@@ -3671,7 +3675,7 @@
         <v>6.4331263300000003</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1044256274</v>
       </c>
@@ -3733,7 +3737,7 @@
         <v>6.398298059</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1044256274</v>
       </c>
@@ -3981,7 +3985,7 @@
         <v>4.7211459700000002</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1044258330</v>
       </c>
@@ -4043,7 +4047,7 @@
         <v>5.2050875769999996</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1044258330</v>
       </c>
@@ -4105,7 +4109,7 @@
         <v>5.2058270999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1044258330</v>
       </c>
@@ -4167,7 +4171,7 @@
         <v>5.3720150679999996</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1044258587</v>
       </c>
@@ -4229,7 +4233,7 @@
         <v>18.693731509999999</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1044258587</v>
       </c>
@@ -4291,7 +4295,7 @@
         <v>18.73249667</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1044258587</v>
       </c>
@@ -4353,7 +4357,7 @@
         <v>18.714106080000001</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1044264482</v>
       </c>
@@ -4415,7 +4419,7 @@
         <v>6.5869735819999997</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1044264482</v>
       </c>
@@ -4477,7 +4481,7 @@
         <v>6.6479189060000001</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1044264482</v>
       </c>
@@ -4539,7 +4543,7 @@
         <v>6.7656691589999998</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1044264739</v>
       </c>
@@ -4601,7 +4605,7 @@
         <v>14.28139039</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1044264739</v>
       </c>
@@ -4663,7 +4667,7 @@
         <v>14.26227604</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1044264739</v>
       </c>
@@ -4725,7 +4729,7 @@
         <v>14.31787525</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1044266538</v>
       </c>
@@ -4787,7 +4791,7 @@
         <v>5.6200414900000002</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1044266538</v>
       </c>
@@ -4849,7 +4853,7 @@
         <v>5.4975522420000003</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1044266538</v>
       </c>
@@ -4911,7 +4915,7 @@
         <v>5.5551328829999997</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1044266795</v>
       </c>
@@ -4973,7 +4977,7 @@
         <v>4.574001687</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1044266795</v>
       </c>
@@ -5035,7 +5039,7 @@
         <v>4.559062634</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1044266795</v>
       </c>
@@ -5097,7 +5101,7 @@
         <v>4.5439209260000002</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1044264498</v>
       </c>
@@ -5159,7 +5163,7 @@
         <v>5.1912580220000004</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1044264498</v>
       </c>
@@ -5221,7 +5225,7 @@
         <v>5.2744712150000002</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1044264498</v>
       </c>
@@ -5283,7 +5287,7 @@
         <v>5.3119421009999996</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1044264755</v>
       </c>
@@ -5345,7 +5349,7 @@
         <v>4.8755126339999997</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1044264755</v>
       </c>
@@ -5407,7 +5411,7 @@
         <v>4.8619389530000001</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1044264755</v>
       </c>
@@ -5469,7 +5473,7 @@
         <v>4.889236178</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -5531,7 +5535,7 @@
         <v>5.3063575710000004</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -5593,7 +5597,7 @@
         <v>5.2306494539999999</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -5655,7 +5659,7 @@
         <v>5.3209266489999996</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1061035787</v>
       </c>
@@ -5717,7 +5721,7 @@
         <v>4.8506907049999999</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1061035787</v>
       </c>
@@ -5779,7 +5783,7 @@
         <v>4.7783915490000002</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1061035787</v>
       </c>
@@ -5841,7 +5845,7 @@
         <v>4.7919477739999996</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1061035794</v>
       </c>
@@ -5903,7 +5907,7 @@
         <v>5.3616740869999999</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1061035794</v>
       </c>
@@ -5965,7 +5969,7 @@
         <v>5.3196051290000002</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1061035794</v>
       </c>
@@ -6213,7 +6217,7 @@
         <v>4.811546206</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -6275,7 +6279,7 @@
         <v>16.433719230000001</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -6337,7 +6341,7 @@
         <v>16.426471299999999</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -6399,7 +6403,7 @@
         <v>16.431570050000001</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1061035803</v>
       </c>
@@ -6461,7 +6465,7 @@
         <v>4.5655369759999997</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1061035803</v>
       </c>
@@ -6523,7 +6527,7 @@
         <v>4.6723914999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1061035803</v>
       </c>
@@ -6585,7 +6589,7 @@
         <v>4.6691145220000001</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1061044002</v>
       </c>
@@ -6647,7 +6651,7 @@
         <v>5.0747935259999997</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1061044002</v>
       </c>
@@ -6709,7 +6713,7 @@
         <v>5.0120690039999998</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1061044002</v>
       </c>
@@ -6771,7 +6775,7 @@
         <v>5.1959706199999998</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1061044003</v>
       </c>
@@ -6833,7 +6837,7 @@
         <v>4.8552270450000004</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1061044003</v>
       </c>
@@ -6895,7 +6899,7 @@
         <v>4.7961669310000001</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1061044003</v>
       </c>
@@ -6957,7 +6961,7 @@
         <v>4.9234126299999996</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -7019,7 +7023,7 @@
         <v>5.4717349149999999</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>5.4742804600000001</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -7143,7 +7147,7 @@
         <v>5.6068905759999996</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1061044011</v>
       </c>
@@ -7205,7 +7209,7 @@
         <v>4.7769116499999997</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1061044011</v>
       </c>
@@ -7267,7 +7271,7 @@
         <v>4.6859034470000003</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1061044011</v>
       </c>
@@ -7329,7 +7333,7 @@
         <v>4.7038197520000002</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -7391,7 +7395,7 @@
         <v>6.2488811359999996</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -7453,7 +7457,7 @@
         <v>6.3783645629999999</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -7515,7 +7519,7 @@
         <v>6.5155110189999998</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1061044019</v>
       </c>
@@ -7577,7 +7581,7 @@
         <v>4.9108786240000004</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1061044019</v>
       </c>
@@ -7639,7 +7643,7 @@
         <v>5.1085914880000001</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1061044019</v>
       </c>
@@ -7701,7 +7705,7 @@
         <v>4.9492299559999999</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1061044026</v>
       </c>
@@ -7763,7 +7767,7 @@
         <v>5.0468798189999999</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1061044026</v>
       </c>
@@ -7825,7 +7829,7 @@
         <v>5.04993626</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1061044026</v>
       </c>
@@ -7887,7 +7891,7 @@
         <v>5.1360206939999999</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1061044027</v>
       </c>
@@ -7949,7 +7953,7 @@
         <v>4.8454408129999997</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1061044027</v>
       </c>
@@ -8011,7 +8015,7 @@
         <v>4.7319271729999999</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1061044027</v>
       </c>
@@ -8073,7 +8077,7 @@
         <v>4.9741140430000002</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1044261386</v>
       </c>
@@ -8135,7 +8139,7 @@
         <v>5.2418713060000002</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1044261386</v>
       </c>
@@ -8197,7 +8201,7 @@
         <v>5.2255579399999998</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1044261386</v>
       </c>
@@ -8259,7 +8263,7 @@
         <v>5.2413604090000003</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1044261643</v>
       </c>
@@ -8321,7 +8325,7 @@
         <v>4.7093953409999996</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1044261643</v>
       </c>
@@ -8383,7 +8387,7 @@
         <v>4.6934434349999998</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1044261643</v>
       </c>
@@ -8445,7 +8449,7 @@
         <v>4.6746373180000003</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1044265490</v>
       </c>
@@ -8507,7 +8511,7 @@
         <v>5.403557846</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1044265490</v>
       </c>
@@ -8569,7 +8573,7 @@
         <v>5.1824850700000002</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1044265490</v>
       </c>
@@ -8817,7 +8821,7 @@
         <v>4.5164299860000003</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1044265498</v>
       </c>
@@ -8879,7 +8883,7 @@
         <v>4.814752511</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1044265498</v>
       </c>
@@ -8941,7 +8945,7 @@
         <v>4.8870431529999996</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1044265498</v>
       </c>
@@ -9003,7 +9007,7 @@
         <v>5.0517422810000001</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>1044265755</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>4.5755871700000004</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1044265755</v>
       </c>
@@ -9127,7 +9131,7 @@
         <v>4.6378535879999996</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1044265755</v>
       </c>
@@ -9189,7 +9193,7 @@
         <v>4.7813951970000002</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1044261410</v>
       </c>
@@ -9251,7 +9255,7 @@
         <v>5.2422059430000001</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1044261410</v>
       </c>
@@ -9313,7 +9317,7 @@
         <v>5.3394151589999996</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1044261410</v>
       </c>
@@ -9375,7 +9379,7 @@
         <v>5.4459614409999997</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1044261667</v>
       </c>
@@ -9437,7 +9441,7 @@
         <v>4.7322796919999996</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1044261667</v>
       </c>
@@ -9499,7 +9503,7 @@
         <v>4.8024735280000002</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1044261667</v>
       </c>
@@ -9561,7 +9565,7 @@
         <v>4.7537016019999996</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1044261418</v>
       </c>
@@ -9623,7 +9627,7 @@
         <v>6.1392784120000004</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1044261418</v>
       </c>
@@ -9685,7 +9689,7 @@
         <v>6.1905166930000002</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1044261418</v>
       </c>
@@ -9747,7 +9751,7 @@
         <v>6.1422118120000002</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1044261675</v>
       </c>
@@ -9809,7 +9813,7 @@
         <v>4.9202152659999996</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1044261675</v>
       </c>
@@ -9871,7 +9875,7 @@
         <v>4.811880844</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1044261675</v>
       </c>
@@ -9933,7 +9937,7 @@
         <v>4.9181452820000002</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1044265522</v>
       </c>
@@ -9995,7 +9999,7 @@
         <v>5.1622343910000001</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1044265522</v>
       </c>
@@ -10057,7 +10061,7 @@
         <v>5.1368577139999996</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1044265522</v>
       </c>
@@ -10119,7 +10123,7 @@
         <v>5.0888342519999998</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>0</v>
       </c>
@@ -10181,7 +10185,7 @@
         <v>6.8522027559999996</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>0</v>
       </c>
@@ -10243,7 +10247,7 @@
         <v>6.7447670869999996</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>0</v>
       </c>
@@ -10305,7 +10309,7 @@
         <v>6.7581823889999999</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1044265530</v>
       </c>
@@ -10367,7 +10371,7 @@
         <v>5.6785557950000003</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1044265530</v>
       </c>
@@ -10429,7 +10433,7 @@
         <v>5.911872217</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1044265530</v>
       </c>
@@ -10491,7 +10495,7 @@
         <v>5.8925292320000002</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1044265787</v>
       </c>
@@ -10553,7 +10557,7 @@
         <v>4.7782327450000004</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1044265787</v>
       </c>
@@ -10615,7 +10619,7 @@
         <v>4.8406933040000002</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1044265787</v>
       </c>
@@ -10677,7 +10681,7 @@
         <v>4.6983144110000001</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1061042954</v>
       </c>
@@ -10739,7 +10743,7 @@
         <v>5.2021013839999997</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1061042954</v>
       </c>
@@ -10801,7 +10805,7 @@
         <v>5.4425967589999997</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1061042954</v>
       </c>
@@ -10863,7 +10867,7 @@
         <v>5.2106806209999998</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1061042955</v>
       </c>
@@ -10925,7 +10929,7 @@
         <v>5.0753576410000001</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1061042955</v>
       </c>
@@ -10987,7 +10991,7 @@
         <v>5.1367253069999999</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1061042955</v>
       </c>
@@ -11049,7 +11053,7 @@
         <v>4.9975616589999996</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1061040914</v>
       </c>
@@ -11111,7 +11115,7 @@
         <v>6.3078620599999997</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1061040914</v>
       </c>
@@ -11173,7 +11177,7 @@
         <v>6.4303253380000003</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1061040914</v>
       </c>
@@ -11421,7 +11425,7 @@
         <v>4.5706983120000002</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1061042970</v>
       </c>
@@ -11483,7 +11487,7 @@
         <v>5.1040815459999997</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1061042970</v>
       </c>
@@ -11545,7 +11549,7 @@
         <v>5.1813576899999996</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1061042970</v>
       </c>
@@ -11607,7 +11611,7 @@
         <v>5.1886771410000003</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1061042971</v>
       </c>
@@ -11669,7 +11673,7 @@
         <v>4.692518711</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1061042971</v>
       </c>
@@ -11731,7 +11735,7 @@
         <v>4.909733364</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1061042971</v>
       </c>
@@ -11793,7 +11797,7 @@
         <v>4.8498890230000002</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1061040930</v>
       </c>
@@ -11855,7 +11859,7 @@
         <v>5.5133104319999999</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1061040930</v>
       </c>
@@ -11917,7 +11921,7 @@
         <v>5.6362139329999996</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1061040930</v>
       </c>
@@ -11979,7 +11983,7 @@
         <v>5.6665765390000002</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1061040931</v>
       </c>
@@ -12041,7 +12045,7 @@
         <v>4.603236914</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1061040931</v>
       </c>
@@ -12103,7 +12107,7 @@
         <v>4.559318083</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1061040931</v>
       </c>
@@ -12165,7 +12169,7 @@
         <v>4.737705418</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1061042986</v>
       </c>
@@ -12227,7 +12231,7 @@
         <v>5.1275649239999996</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1061042986</v>
       </c>
@@ -12289,7 +12293,7 @@
         <v>5.1931521719999996</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1061042986</v>
       </c>
@@ -12351,7 +12355,7 @@
         <v>5.4410376720000002</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1061042987</v>
       </c>
@@ -12413,7 +12417,7 @@
         <v>5.2551452599999999</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1061042987</v>
       </c>
@@ -12475,7 +12479,7 @@
         <v>5.0567541800000004</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>1061042987</v>
       </c>
@@ -12537,7 +12541,7 @@
         <v>5.0159360680000002</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1061040946</v>
       </c>
@@ -12599,7 +12603,7 @@
         <v>5.3729397910000003</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1061040946</v>
       </c>
@@ -12661,7 +12665,7 @@
         <v>5.0709443429999999</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1061040946</v>
       </c>
@@ -12723,7 +12727,7 @@
         <v>5.1505280390000001</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1061040947</v>
       </c>
@@ -12785,7 +12789,7 @@
         <v>5.132435901</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1061040947</v>
       </c>
@@ -12847,7 +12851,7 @@
         <v>5.0672535390000002</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1061040947</v>
       </c>
@@ -12909,7 +12913,7 @@
         <v>5.1821150950000003</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1044265490</v>
       </c>
@@ -12971,7 +12975,7 @@
         <v>5.63446113</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1044265490</v>
       </c>
@@ -13033,7 +13037,7 @@
         <v>5.4609447720000004</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1044265490</v>
       </c>
@@ -13281,7 +13285,7 @@
         <v>4.6363736900000001</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>1044265498</v>
       </c>
@@ -13343,7 +13347,7 @@
         <v>5.275422335</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1044265498</v>
       </c>
@@ -13405,7 +13409,7 @@
         <v>5.2200176889999996</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>1044265498</v>
       </c>
@@ -13467,7 +13471,7 @@
         <v>5.1278995619999996</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1044265755</v>
       </c>
@@ -13529,7 +13533,7 @@
         <v>4.7187145270000004</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>1044265755</v>
       </c>
@@ -13591,7 +13595,7 @@
         <v>4.6164844719999998</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>1044265755</v>
       </c>
@@ -13653,7 +13657,7 @@
         <v>4.7235063139999998</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>1044265506</v>
       </c>
@@ -13715,7 +13719,7 @@
         <v>4.892371808</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1044265506</v>
       </c>
@@ -13777,7 +13781,7 @@
         <v>5.0025914399999998</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1044265506</v>
       </c>
@@ -13839,7 +13843,7 @@
         <v>4.8910771100000003</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1044265763</v>
       </c>
@@ -13901,7 +13905,7 @@
         <v>18.698954579999999</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1044265763</v>
       </c>
@@ -13963,7 +13967,7 @@
         <v>18.68646485</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1044265763</v>
       </c>
@@ -14025,7 +14029,7 @@
         <v>18.69080748</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1044265514</v>
       </c>
@@ -14087,7 +14091,7 @@
         <v>5.5338429549999999</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1044265514</v>
       </c>
@@ -14149,7 +14153,7 @@
         <v>5.4554040940000004</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1044265514</v>
       </c>
@@ -14211,7 +14215,7 @@
         <v>5.5779465610000001</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1044265771</v>
       </c>
@@ -14273,7 +14277,7 @@
         <v>4.9546825029999999</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1044265771</v>
       </c>
@@ -14335,7 +14339,7 @@
         <v>5.0181469749999996</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1044265771</v>
       </c>
@@ -14398,6 +14402,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T217" xr:uid="{99B28BD6-0AE5-4BDE-8C7D-DF8C3B7D02E6}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="19"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>